<commit_message>
added cars 10 + 11
</commit_message>
<xml_diff>
--- a/devData/H77Dyno.xlsx
+++ b/devData/H77Dyno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\SQL\Halle77Dyno\devData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EDD834-3291-4828-8B9D-1A9A04E83B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6537C363-ABE9-481D-8C36-2D2E16C0187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5738,8 +5738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="D427" sqref="D427:T427"/>
+    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="D396" sqref="D396:T396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16149,21 +16149,33 @@
       <c r="C396" s="4">
         <v>1</v>
       </c>
-      <c r="D396" t="s">
+      <c r="D396" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="E396" s="4">
+      <c r="E396" s="20">
         <v>944</v>
       </c>
-      <c r="F396" s="2" t="s">
+      <c r="F396" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="L396" s="3">
+      <c r="G396" s="14"/>
+      <c r="H396" s="16"/>
+      <c r="I396" s="14"/>
+      <c r="J396" s="16"/>
+      <c r="K396" s="14"/>
+      <c r="L396" s="16">
         <v>163</v>
       </c>
-      <c r="Q396" s="3" t="s">
+      <c r="M396" s="14"/>
+      <c r="N396" s="16"/>
+      <c r="O396" s="14"/>
+      <c r="P396" s="14"/>
+      <c r="Q396" s="16" t="s">
         <v>1232</v>
       </c>
+      <c r="R396" s="16"/>
+      <c r="S396" s="16"/>
+      <c r="T396" s="16"/>
       <c r="X396" t="s">
         <v>146</v>
       </c>
@@ -16561,22 +16573,33 @@
       <c r="C410" s="4">
         <v>1</v>
       </c>
-      <c r="D410" t="s">
+      <c r="D410" s="6" t="s">
         <v>841</v>
       </c>
-      <c r="E410" s="4" t="s">
+      <c r="E410" s="5" t="s">
         <v>842</v>
       </c>
-      <c r="F410" s="2" t="s">
+      <c r="F410" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="G410" t="s">
+      <c r="G410" s="6" t="s">
         <v>843</v>
       </c>
-      <c r="L410" s="3">
+      <c r="H410" s="8"/>
+      <c r="I410" s="6"/>
+      <c r="J410" s="8"/>
+      <c r="K410" s="6"/>
+      <c r="L410" s="8">
         <v>120</v>
       </c>
-      <c r="T410" s="3" t="s">
+      <c r="M410" s="6"/>
+      <c r="N410" s="8"/>
+      <c r="O410" s="6"/>
+      <c r="P410" s="6"/>
+      <c r="Q410" s="8"/>
+      <c r="R410" s="8"/>
+      <c r="S410" s="8"/>
+      <c r="T410" s="8" t="s">
         <v>1217</v>
       </c>
       <c r="X410" t="s">
@@ -16587,22 +16610,33 @@
       <c r="C411" s="4">
         <v>2</v>
       </c>
-      <c r="D411" t="s">
+      <c r="D411" s="6" t="s">
         <v>841</v>
       </c>
-      <c r="E411" s="4" t="s">
+      <c r="E411" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="F411" s="2" t="s">
+      <c r="F411" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="G411" t="s">
+      <c r="G411" s="6" t="s">
         <v>844</v>
       </c>
-      <c r="L411" s="3">
+      <c r="H411" s="8"/>
+      <c r="I411" s="6"/>
+      <c r="J411" s="8"/>
+      <c r="K411" s="6"/>
+      <c r="L411" s="8">
         <v>150</v>
       </c>
-      <c r="T411" s="3" t="s">
+      <c r="M411" s="6"/>
+      <c r="N411" s="8"/>
+      <c r="O411" s="6"/>
+      <c r="P411" s="6"/>
+      <c r="Q411" s="8"/>
+      <c r="R411" s="8"/>
+      <c r="S411" s="8"/>
+      <c r="T411" s="8" t="s">
         <v>1218</v>
       </c>
       <c r="X411" t="s">
@@ -16613,16 +16647,29 @@
       <c r="C412" s="4">
         <v>3</v>
       </c>
-      <c r="D412" t="s">
+      <c r="D412" s="6" t="s">
         <v>841</v>
       </c>
-      <c r="E412" s="4" t="s">
+      <c r="E412" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="Q412" s="3" t="s">
+      <c r="F412" s="7"/>
+      <c r="G412" s="6"/>
+      <c r="H412" s="8"/>
+      <c r="I412" s="6"/>
+      <c r="J412" s="8"/>
+      <c r="K412" s="6"/>
+      <c r="L412" s="8"/>
+      <c r="M412" s="6"/>
+      <c r="N412" s="8"/>
+      <c r="O412" s="6"/>
+      <c r="P412" s="6"/>
+      <c r="Q412" s="8" t="s">
         <v>1211</v>
       </c>
-      <c r="T412" s="3" t="s">
+      <c r="R412" s="8"/>
+      <c r="S412" s="8"/>
+      <c r="T412" s="8" t="s">
         <v>1126</v>
       </c>
       <c r="X412" t="s">
@@ -16633,25 +16680,35 @@
       <c r="C413" s="4">
         <v>4</v>
       </c>
-      <c r="D413" t="s">
+      <c r="D413" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E413" s="4" t="s">
+      <c r="E413" s="5" t="s">
         <v>846</v>
       </c>
-      <c r="F413" s="2" t="s">
+      <c r="F413" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="K413" t="s">
+      <c r="G413" s="6"/>
+      <c r="H413" s="8"/>
+      <c r="I413" s="6"/>
+      <c r="J413" s="8"/>
+      <c r="K413" s="6" t="s">
         <v>845</v>
       </c>
-      <c r="L413" s="3">
+      <c r="L413" s="8">
         <v>231</v>
       </c>
-      <c r="Q413" s="3" t="s">
+      <c r="M413" s="6"/>
+      <c r="N413" s="8"/>
+      <c r="O413" s="6"/>
+      <c r="P413" s="6"/>
+      <c r="Q413" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T413" s="3" t="s">
+      <c r="R413" s="8"/>
+      <c r="S413" s="8"/>
+      <c r="T413" s="8" t="s">
         <v>1219</v>
       </c>
       <c r="X413" t="s">
@@ -16662,25 +16719,35 @@
       <c r="C414" s="4">
         <v>5</v>
       </c>
-      <c r="D414" t="s">
+      <c r="D414" s="6" t="s">
         <v>841</v>
       </c>
-      <c r="E414" s="4" t="s">
+      <c r="E414" s="5" t="s">
         <v>847</v>
       </c>
-      <c r="F414" s="2" t="s">
+      <c r="F414" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="J414" s="3">
+      <c r="G414" s="6"/>
+      <c r="H414" s="8"/>
+      <c r="I414" s="6"/>
+      <c r="J414" s="8">
         <v>5</v>
       </c>
-      <c r="L414" s="3">
+      <c r="K414" s="6"/>
+      <c r="L414" s="8">
         <v>150</v>
       </c>
-      <c r="Q414" s="3" t="s">
+      <c r="M414" s="6"/>
+      <c r="N414" s="8"/>
+      <c r="O414" s="6"/>
+      <c r="P414" s="6"/>
+      <c r="Q414" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T414" s="3" t="s">
+      <c r="R414" s="8"/>
+      <c r="S414" s="8"/>
+      <c r="T414" s="8" t="s">
         <v>1220</v>
       </c>
       <c r="X414" t="s">
@@ -16691,25 +16758,35 @@
       <c r="C415" s="4">
         <v>6</v>
       </c>
-      <c r="D415" t="s">
+      <c r="D415" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E415" s="4" t="s">
+      <c r="E415" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="F415" s="2" t="s">
+      <c r="F415" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="L415" s="3">
+      <c r="G415" s="6"/>
+      <c r="H415" s="8"/>
+      <c r="I415" s="6"/>
+      <c r="J415" s="8"/>
+      <c r="K415" s="6"/>
+      <c r="L415" s="8">
         <v>231</v>
       </c>
-      <c r="M415" s="1">
+      <c r="M415" s="9">
         <v>76000</v>
       </c>
-      <c r="Q415" s="3" t="s">
+      <c r="N415" s="8"/>
+      <c r="O415" s="6"/>
+      <c r="P415" s="6"/>
+      <c r="Q415" s="8" t="s">
         <v>1212</v>
       </c>
-      <c r="T415" s="3" t="s">
+      <c r="R415" s="8"/>
+      <c r="S415" s="8"/>
+      <c r="T415" s="8" t="s">
         <v>1221</v>
       </c>
       <c r="X415" t="s">
@@ -16729,19 +16806,31 @@
       <c r="C416" s="4">
         <v>7</v>
       </c>
-      <c r="D416" t="s">
+      <c r="D416" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E416" s="4" t="s">
+      <c r="E416" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="G416" t="s">
+      <c r="F416" s="7"/>
+      <c r="G416" s="6" t="s">
         <v>852</v>
       </c>
-      <c r="Q416" s="3" t="s">
+      <c r="H416" s="8"/>
+      <c r="I416" s="6"/>
+      <c r="J416" s="8"/>
+      <c r="K416" s="6"/>
+      <c r="L416" s="8"/>
+      <c r="M416" s="6"/>
+      <c r="N416" s="8"/>
+      <c r="O416" s="6"/>
+      <c r="P416" s="6"/>
+      <c r="Q416" s="8" t="s">
         <v>1213</v>
       </c>
-      <c r="T416" s="3" t="s">
+      <c r="R416" s="8"/>
+      <c r="S416" s="8"/>
+      <c r="T416" s="8" t="s">
         <v>1222</v>
       </c>
       <c r="X416" t="s">
@@ -16752,22 +16841,33 @@
       <c r="C417" s="4">
         <v>8</v>
       </c>
-      <c r="D417" t="s">
+      <c r="D417" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E417" s="4" t="s">
+      <c r="E417" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="F417" s="2" t="s">
+      <c r="F417" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="L417" s="3">
+      <c r="G417" s="6"/>
+      <c r="H417" s="8"/>
+      <c r="I417" s="6"/>
+      <c r="J417" s="8"/>
+      <c r="K417" s="6"/>
+      <c r="L417" s="8">
         <v>90</v>
       </c>
-      <c r="Q417" s="3" t="s">
+      <c r="M417" s="6"/>
+      <c r="N417" s="8"/>
+      <c r="O417" s="6"/>
+      <c r="P417" s="6"/>
+      <c r="Q417" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T417" s="3" t="s">
+      <c r="R417" s="8"/>
+      <c r="S417" s="8"/>
+      <c r="T417" s="8" t="s">
         <v>1223</v>
       </c>
     </row>
@@ -16775,25 +16875,35 @@
       <c r="C418" s="4">
         <v>9</v>
       </c>
-      <c r="D418" t="s">
+      <c r="D418" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E418" s="4" t="s">
+      <c r="E418" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="F418" s="2" t="s">
+      <c r="F418" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L418" s="3">
+      <c r="G418" s="6"/>
+      <c r="H418" s="8"/>
+      <c r="I418" s="6"/>
+      <c r="J418" s="8"/>
+      <c r="K418" s="6"/>
+      <c r="L418" s="8">
         <v>88</v>
       </c>
-      <c r="N418" s="3">
+      <c r="M418" s="6"/>
+      <c r="N418" s="8">
         <v>1992</v>
       </c>
-      <c r="Q418" s="3" t="s">
+      <c r="O418" s="6"/>
+      <c r="P418" s="6"/>
+      <c r="Q418" s="8" t="s">
         <v>1214</v>
       </c>
-      <c r="T418" s="3" t="s">
+      <c r="R418" s="8"/>
+      <c r="S418" s="8"/>
+      <c r="T418" s="8" t="s">
         <v>1224</v>
       </c>
       <c r="X418" t="s">
@@ -16804,25 +16914,35 @@
       <c r="C419" s="4">
         <v>10</v>
       </c>
-      <c r="D419" t="s">
+      <c r="D419" s="6" t="s">
         <v>841</v>
       </c>
-      <c r="E419" s="4" t="s">
+      <c r="E419" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="F419" s="2" t="s">
+      <c r="F419" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="L419" s="3">
+      <c r="G419" s="6"/>
+      <c r="H419" s="8"/>
+      <c r="I419" s="6"/>
+      <c r="J419" s="8"/>
+      <c r="K419" s="6"/>
+      <c r="L419" s="8">
         <v>75</v>
       </c>
-      <c r="M419" s="1">
+      <c r="M419" s="9">
         <v>214000</v>
       </c>
-      <c r="Q419" s="3" t="s">
+      <c r="N419" s="8"/>
+      <c r="O419" s="6"/>
+      <c r="P419" s="6"/>
+      <c r="Q419" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T419" s="3" t="s">
+      <c r="R419" s="8"/>
+      <c r="S419" s="8"/>
+      <c r="T419" s="8" t="s">
         <v>1225</v>
       </c>
       <c r="X419" t="s">
@@ -16833,19 +16953,31 @@
       <c r="C420" s="4">
         <v>11</v>
       </c>
-      <c r="D420" t="s">
+      <c r="D420" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E420" s="4" t="s">
+      <c r="E420" s="5" t="s">
         <v>851</v>
       </c>
-      <c r="L420" s="3">
+      <c r="F420" s="7"/>
+      <c r="G420" s="6"/>
+      <c r="H420" s="8"/>
+      <c r="I420" s="6"/>
+      <c r="J420" s="8"/>
+      <c r="K420" s="6"/>
+      <c r="L420" s="8">
         <v>150</v>
       </c>
-      <c r="Q420" s="3" t="s">
+      <c r="M420" s="6"/>
+      <c r="N420" s="8"/>
+      <c r="O420" s="6"/>
+      <c r="P420" s="6"/>
+      <c r="Q420" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T420" s="3" t="s">
+      <c r="R420" s="8"/>
+      <c r="S420" s="8"/>
+      <c r="T420" s="8" t="s">
         <v>1226</v>
       </c>
       <c r="AA420" t="s">
@@ -16856,25 +16988,35 @@
       <c r="C421" s="4">
         <v>12</v>
       </c>
-      <c r="D421" t="s">
+      <c r="D421" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E421" s="4">
+      <c r="E421" s="5">
         <v>90</v>
       </c>
-      <c r="F421" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="K421" t="s">
+      <c r="F421" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="G421" s="6"/>
+      <c r="H421" s="8"/>
+      <c r="I421" s="6"/>
+      <c r="J421" s="8"/>
+      <c r="K421" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="L421" s="3">
+      <c r="L421" s="8">
         <v>136</v>
       </c>
-      <c r="Q421" s="3" t="s">
+      <c r="M421" s="6"/>
+      <c r="N421" s="8"/>
+      <c r="O421" s="6"/>
+      <c r="P421" s="6"/>
+      <c r="Q421" s="8" t="s">
         <v>1215</v>
       </c>
-      <c r="T421" s="3" t="s">
+      <c r="R421" s="8"/>
+      <c r="S421" s="8"/>
+      <c r="T421" s="8" t="s">
         <v>1227</v>
       </c>
       <c r="X421" t="s">
@@ -16894,22 +17036,33 @@
       <c r="C422" s="4">
         <v>13</v>
       </c>
-      <c r="D422" t="s">
+      <c r="D422" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E422" s="4" t="s">
+      <c r="E422" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="J422" s="3">
+      <c r="F422" s="7"/>
+      <c r="G422" s="6"/>
+      <c r="H422" s="8"/>
+      <c r="I422" s="6"/>
+      <c r="J422" s="8">
         <v>6</v>
       </c>
-      <c r="L422" s="3">
+      <c r="K422" s="6"/>
+      <c r="L422" s="8">
         <v>271</v>
       </c>
-      <c r="Q422" s="3" t="s">
+      <c r="M422" s="6"/>
+      <c r="N422" s="8"/>
+      <c r="O422" s="6"/>
+      <c r="P422" s="6"/>
+      <c r="Q422" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T422" s="3" t="s">
+      <c r="R422" s="8"/>
+      <c r="S422" s="8"/>
+      <c r="T422" s="8" t="s">
         <v>1228</v>
       </c>
       <c r="X422" t="s">
@@ -16920,25 +17073,35 @@
       <c r="C423" s="4">
         <v>14</v>
       </c>
-      <c r="D423" t="s">
+      <c r="D423" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="E423" s="4" t="s">
+      <c r="E423" s="5" t="s">
         <v>859</v>
       </c>
-      <c r="F423" s="2" t="s">
+      <c r="F423" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G423" t="s">
+      <c r="G423" s="6" t="s">
         <v>639</v>
       </c>
-      <c r="L423" s="3">
+      <c r="H423" s="8"/>
+      <c r="I423" s="6"/>
+      <c r="J423" s="8"/>
+      <c r="K423" s="6"/>
+      <c r="L423" s="8">
         <v>200</v>
       </c>
-      <c r="Q423" s="3" t="s">
+      <c r="M423" s="6"/>
+      <c r="N423" s="8"/>
+      <c r="O423" s="6"/>
+      <c r="P423" s="6"/>
+      <c r="Q423" s="8" t="s">
         <v>1216</v>
       </c>
-      <c r="T423" s="3" t="s">
+      <c r="R423" s="8"/>
+      <c r="S423" s="8"/>
+      <c r="T423" s="8" t="s">
         <v>1229</v>
       </c>
       <c r="X423" t="s">
@@ -16958,13 +17121,27 @@
       <c r="C424" s="4">
         <v>15</v>
       </c>
-      <c r="D424" t="s">
+      <c r="D424" s="6" t="s">
         <v>860</v>
       </c>
-      <c r="L424" s="3">
+      <c r="E424" s="5"/>
+      <c r="F424" s="7"/>
+      <c r="G424" s="6"/>
+      <c r="H424" s="8"/>
+      <c r="I424" s="6"/>
+      <c r="J424" s="8"/>
+      <c r="K424" s="6"/>
+      <c r="L424" s="8">
         <v>160</v>
       </c>
-      <c r="T424" s="3" t="s">
+      <c r="M424" s="6"/>
+      <c r="N424" s="8"/>
+      <c r="O424" s="6"/>
+      <c r="P424" s="6"/>
+      <c r="Q424" s="8"/>
+      <c r="R424" s="8"/>
+      <c r="S424" s="8"/>
+      <c r="T424" s="8" t="s">
         <v>1230</v>
       </c>
       <c r="X424" t="s">
@@ -16975,22 +17152,33 @@
       <c r="C425" s="4">
         <v>16</v>
       </c>
-      <c r="D425" t="s">
+      <c r="D425" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E425" s="4" t="s">
+      <c r="E425" s="5" t="s">
         <v>861</v>
       </c>
-      <c r="F425" s="2" t="s">
+      <c r="F425" s="7" t="s">
         <v>862</v>
       </c>
-      <c r="G425" t="s">
+      <c r="G425" s="6" t="s">
         <v>863</v>
       </c>
-      <c r="L425" s="3">
+      <c r="H425" s="8"/>
+      <c r="I425" s="6"/>
+      <c r="J425" s="8"/>
+      <c r="K425" s="6"/>
+      <c r="L425" s="8">
         <v>39</v>
       </c>
-      <c r="T425" s="3" t="s">
+      <c r="M425" s="6"/>
+      <c r="N425" s="8"/>
+      <c r="O425" s="6"/>
+      <c r="P425" s="6"/>
+      <c r="Q425" s="8"/>
+      <c r="R425" s="8"/>
+      <c r="S425" s="8"/>
+      <c r="T425" s="8" t="s">
         <v>1231</v>
       </c>
       <c r="X425" t="s">
@@ -17006,33 +17194,33 @@
       <c r="C427" s="4">
         <v>1</v>
       </c>
-      <c r="D427" s="14" t="s">
+      <c r="D427" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E427" s="20" t="s">
+      <c r="E427" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="F427" s="15" t="s">
+      <c r="F427" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G427" s="14" t="s">
+      <c r="G427" s="6" t="s">
         <v>816</v>
       </c>
-      <c r="H427" s="16"/>
-      <c r="I427" s="14"/>
-      <c r="J427" s="16"/>
-      <c r="K427" s="14"/>
-      <c r="L427" s="16">
+      <c r="H427" s="8"/>
+      <c r="I427" s="6"/>
+      <c r="J427" s="8"/>
+      <c r="K427" s="6"/>
+      <c r="L427" s="8">
         <v>150</v>
       </c>
-      <c r="M427" s="14"/>
-      <c r="N427" s="16"/>
-      <c r="O427" s="14"/>
-      <c r="P427" s="14"/>
-      <c r="Q427" s="16"/>
-      <c r="R427" s="16"/>
-      <c r="S427" s="16"/>
-      <c r="T427" s="16" t="s">
+      <c r="M427" s="6"/>
+      <c r="N427" s="8"/>
+      <c r="O427" s="6"/>
+      <c r="P427" s="6"/>
+      <c r="Q427" s="8"/>
+      <c r="R427" s="8"/>
+      <c r="S427" s="8"/>
+      <c r="T427" s="8" t="s">
         <v>1192</v>
       </c>
       <c r="X427" t="s">
@@ -17043,19 +17231,31 @@
       <c r="C428" s="4">
         <v>2</v>
       </c>
-      <c r="D428" t="s">
+      <c r="D428" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E428" s="4" t="s">
+      <c r="E428" s="5" t="s">
         <v>817</v>
       </c>
-      <c r="F428" s="2" t="s">
+      <c r="F428" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L428" s="3">
+      <c r="G428" s="6"/>
+      <c r="H428" s="8"/>
+      <c r="I428" s="6"/>
+      <c r="J428" s="8"/>
+      <c r="K428" s="6"/>
+      <c r="L428" s="8">
         <v>150</v>
       </c>
-      <c r="T428" s="3" t="s">
+      <c r="M428" s="6"/>
+      <c r="N428" s="8"/>
+      <c r="O428" s="6"/>
+      <c r="P428" s="6"/>
+      <c r="Q428" s="8"/>
+      <c r="R428" s="8"/>
+      <c r="S428" s="8"/>
+      <c r="T428" s="8" t="s">
         <v>1193</v>
       </c>
     </row>
@@ -17063,22 +17263,33 @@
       <c r="C429" s="4">
         <v>3</v>
       </c>
-      <c r="D429" t="s">
+      <c r="D429" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E429" s="4" t="s">
+      <c r="E429" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="F429" s="2" t="s">
+      <c r="F429" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="G429" t="s">
+      <c r="G429" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="L429" s="3">
+      <c r="H429" s="8"/>
+      <c r="I429" s="6"/>
+      <c r="J429" s="8"/>
+      <c r="K429" s="6"/>
+      <c r="L429" s="8">
         <v>98</v>
       </c>
-      <c r="T429" s="3" t="s">
+      <c r="M429" s="6"/>
+      <c r="N429" s="8"/>
+      <c r="O429" s="6"/>
+      <c r="P429" s="6"/>
+      <c r="Q429" s="8"/>
+      <c r="R429" s="8"/>
+      <c r="S429" s="8"/>
+      <c r="T429" s="8" t="s">
         <v>1194</v>
       </c>
       <c r="X429" t="s">
@@ -17089,25 +17300,35 @@
       <c r="C430" s="4">
         <v>4</v>
       </c>
-      <c r="D430" t="s">
+      <c r="D430" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E430" s="4" t="s">
+      <c r="E430" s="5" t="s">
         <v>596</v>
       </c>
-      <c r="F430" s="2" t="s">
+      <c r="F430" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="J430" s="3">
+      <c r="G430" s="6"/>
+      <c r="H430" s="8"/>
+      <c r="I430" s="6"/>
+      <c r="J430" s="8">
         <v>5</v>
       </c>
-      <c r="L430" s="3">
+      <c r="K430" s="6"/>
+      <c r="L430" s="8">
         <v>133</v>
       </c>
-      <c r="Q430" s="3" t="s">
+      <c r="M430" s="6"/>
+      <c r="N430" s="8"/>
+      <c r="O430" s="6"/>
+      <c r="P430" s="6"/>
+      <c r="Q430" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="T430" s="3" t="s">
+      <c r="R430" s="8"/>
+      <c r="S430" s="8"/>
+      <c r="T430" s="8" t="s">
         <v>1195</v>
       </c>
       <c r="X430" t="s">
@@ -17118,25 +17339,35 @@
       <c r="C431" s="4">
         <v>5</v>
       </c>
-      <c r="D431" t="s">
+      <c r="D431" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="E431" s="4" t="s">
+      <c r="E431" s="5" t="s">
         <v>819</v>
       </c>
-      <c r="F431" s="2" t="s">
+      <c r="F431" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="G431" t="s">
+      <c r="G431" s="6" t="s">
         <v>829</v>
       </c>
-      <c r="L431" s="3">
+      <c r="H431" s="8"/>
+      <c r="I431" s="6"/>
+      <c r="J431" s="8"/>
+      <c r="K431" s="6"/>
+      <c r="L431" s="8">
         <v>90</v>
       </c>
-      <c r="Q431" s="3" t="s">
+      <c r="M431" s="6"/>
+      <c r="N431" s="8"/>
+      <c r="O431" s="6"/>
+      <c r="P431" s="6"/>
+      <c r="Q431" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="T431" s="3" t="s">
+      <c r="R431" s="8"/>
+      <c r="S431" s="8"/>
+      <c r="T431" s="8" t="s">
         <v>1196</v>
       </c>
     </row>
@@ -17144,22 +17375,33 @@
       <c r="C432" s="4">
         <v>6</v>
       </c>
-      <c r="D432" t="s">
+      <c r="D432" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E432" s="4" t="s">
+      <c r="E432" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="F432" s="2" t="s">
+      <c r="F432" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L432" s="3">
+      <c r="G432" s="6"/>
+      <c r="H432" s="8"/>
+      <c r="I432" s="6"/>
+      <c r="J432" s="8"/>
+      <c r="K432" s="6"/>
+      <c r="L432" s="8">
         <v>90</v>
       </c>
-      <c r="Q432" s="3" t="s">
+      <c r="M432" s="6"/>
+      <c r="N432" s="8"/>
+      <c r="O432" s="6"/>
+      <c r="P432" s="6"/>
+      <c r="Q432" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T432" s="3" t="s">
+      <c r="R432" s="8"/>
+      <c r="S432" s="8"/>
+      <c r="T432" s="8" t="s">
         <v>1197</v>
       </c>
       <c r="X432" t="s">
@@ -17179,22 +17421,33 @@
       <c r="C433" s="4">
         <v>7</v>
       </c>
-      <c r="D433" t="s">
+      <c r="D433" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E433" s="4" t="s">
+      <c r="E433" s="5" t="s">
         <v>825</v>
       </c>
-      <c r="F433" s="2" t="s">
+      <c r="F433" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L433" s="3">
+      <c r="G433" s="6"/>
+      <c r="H433" s="8"/>
+      <c r="I433" s="6"/>
+      <c r="J433" s="8"/>
+      <c r="K433" s="6"/>
+      <c r="L433" s="8">
         <v>200</v>
       </c>
-      <c r="Q433" s="3" t="s">
+      <c r="M433" s="6"/>
+      <c r="N433" s="8"/>
+      <c r="O433" s="6"/>
+      <c r="P433" s="6"/>
+      <c r="Q433" s="8" t="s">
         <v>1190</v>
       </c>
-      <c r="T433" s="3" t="s">
+      <c r="R433" s="8"/>
+      <c r="S433" s="8"/>
+      <c r="T433" s="8" t="s">
         <v>1198</v>
       </c>
       <c r="X433" t="s">
@@ -17214,22 +17467,33 @@
       <c r="C434" s="4">
         <v>8</v>
       </c>
-      <c r="D434" t="s">
+      <c r="D434" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E434" s="4">
+      <c r="E434" s="5">
         <v>996</v>
       </c>
-      <c r="F434" s="2" t="s">
+      <c r="F434" s="7" t="s">
         <v>826</v>
       </c>
-      <c r="L434" s="3">
+      <c r="G434" s="6"/>
+      <c r="H434" s="8"/>
+      <c r="I434" s="6"/>
+      <c r="J434" s="8"/>
+      <c r="K434" s="6"/>
+      <c r="L434" s="8">
         <v>300</v>
       </c>
-      <c r="Q434" s="3" t="s">
+      <c r="M434" s="6"/>
+      <c r="N434" s="8"/>
+      <c r="O434" s="6"/>
+      <c r="P434" s="6"/>
+      <c r="Q434" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T434" s="3" t="s">
+      <c r="R434" s="8"/>
+      <c r="S434" s="8"/>
+      <c r="T434" s="8" t="s">
         <v>1199</v>
       </c>
       <c r="X434" t="s">
@@ -17240,25 +17504,35 @@
       <c r="C435" s="4">
         <v>9</v>
       </c>
-      <c r="D435" t="s">
+      <c r="D435" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E435" s="4" t="s">
+      <c r="E435" s="5" t="s">
         <v>827</v>
       </c>
-      <c r="F435" s="2" t="s">
+      <c r="F435" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="G435" t="s">
+      <c r="G435" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="L435" s="3">
+      <c r="H435" s="8"/>
+      <c r="I435" s="6"/>
+      <c r="J435" s="8"/>
+      <c r="K435" s="6"/>
+      <c r="L435" s="8">
         <v>131</v>
       </c>
-      <c r="Q435" s="3" t="s">
+      <c r="M435" s="6"/>
+      <c r="N435" s="8"/>
+      <c r="O435" s="6"/>
+      <c r="P435" s="6"/>
+      <c r="Q435" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T435" s="3" t="s">
+      <c r="R435" s="8"/>
+      <c r="S435" s="8"/>
+      <c r="T435" s="8" t="s">
         <v>1200</v>
       </c>
     </row>
@@ -17266,22 +17540,33 @@
       <c r="C436" s="4">
         <v>10</v>
       </c>
-      <c r="D436" t="s">
+      <c r="D436" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E436" s="4" t="s">
+      <c r="E436" s="5" t="s">
         <v>828</v>
       </c>
-      <c r="F436" s="2" t="s">
+      <c r="F436" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="L436" s="3">
+      <c r="G436" s="6"/>
+      <c r="H436" s="8"/>
+      <c r="I436" s="6"/>
+      <c r="J436" s="8"/>
+      <c r="K436" s="6"/>
+      <c r="L436" s="8">
         <v>150</v>
       </c>
-      <c r="Q436" s="3" t="s">
+      <c r="M436" s="6"/>
+      <c r="N436" s="8"/>
+      <c r="O436" s="6"/>
+      <c r="P436" s="6"/>
+      <c r="Q436" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T436" s="3" t="s">
+      <c r="R436" s="8"/>
+      <c r="S436" s="8"/>
+      <c r="T436" s="8" t="s">
         <v>1201</v>
       </c>
     </row>
@@ -17289,25 +17574,35 @@
       <c r="C437" s="4">
         <v>11</v>
       </c>
-      <c r="D437" t="s">
+      <c r="D437" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E437" s="4" t="s">
+      <c r="E437" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="F437" s="2" t="s">
+      <c r="F437" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="G437" t="s">
+      <c r="G437" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="L437" s="3">
+      <c r="H437" s="8"/>
+      <c r="I437" s="6"/>
+      <c r="J437" s="8"/>
+      <c r="K437" s="6"/>
+      <c r="L437" s="8">
         <v>75</v>
       </c>
-      <c r="Q437" s="3" t="s">
+      <c r="M437" s="6"/>
+      <c r="N437" s="8"/>
+      <c r="O437" s="6"/>
+      <c r="P437" s="6"/>
+      <c r="Q437" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T437" s="3" t="s">
+      <c r="R437" s="8"/>
+      <c r="S437" s="8"/>
+      <c r="T437" s="8" t="s">
         <v>1202</v>
       </c>
       <c r="X437" t="s">
@@ -17318,22 +17613,33 @@
       <c r="C438" s="4">
         <v>12</v>
       </c>
-      <c r="D438" t="s">
+      <c r="D438" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E438" s="4" t="s">
+      <c r="E438" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="F438" s="2" t="s">
+      <c r="F438" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L438" s="3">
+      <c r="G438" s="6"/>
+      <c r="H438" s="8"/>
+      <c r="I438" s="6"/>
+      <c r="J438" s="8"/>
+      <c r="K438" s="6"/>
+      <c r="L438" s="8">
         <v>98</v>
       </c>
-      <c r="Q438" s="3" t="s">
+      <c r="M438" s="6"/>
+      <c r="N438" s="8"/>
+      <c r="O438" s="6"/>
+      <c r="P438" s="6"/>
+      <c r="Q438" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T438" s="3" t="s">
+      <c r="R438" s="8"/>
+      <c r="S438" s="8"/>
+      <c r="T438" s="8" t="s">
         <v>1203</v>
       </c>
       <c r="X438" t="s">
@@ -17353,25 +17659,35 @@
       <c r="C439" s="4">
         <v>13</v>
       </c>
-      <c r="D439" t="s">
+      <c r="D439" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E439" s="4" t="s">
+      <c r="E439" s="5" t="s">
         <v>834</v>
       </c>
-      <c r="F439" s="2" t="s">
+      <c r="F439" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L439" s="3">
+      <c r="G439" s="6"/>
+      <c r="H439" s="8"/>
+      <c r="I439" s="6"/>
+      <c r="J439" s="8"/>
+      <c r="K439" s="6"/>
+      <c r="L439" s="8">
         <v>112</v>
       </c>
-      <c r="N439" s="3">
+      <c r="M439" s="6"/>
+      <c r="N439" s="8">
         <v>1983</v>
       </c>
-      <c r="Q439" s="3" t="s">
+      <c r="O439" s="6"/>
+      <c r="P439" s="6"/>
+      <c r="Q439" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="T439" s="3" t="s">
+      <c r="R439" s="8"/>
+      <c r="S439" s="8"/>
+      <c r="T439" s="8" t="s">
         <v>1204</v>
       </c>
       <c r="X439" t="s">
@@ -17382,22 +17698,33 @@
       <c r="C440" s="4">
         <v>14</v>
       </c>
-      <c r="D440" t="s">
+      <c r="D440" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E440" s="4">
+      <c r="E440" s="5">
         <v>90</v>
       </c>
-      <c r="F440" s="2" t="s">
+      <c r="F440" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="L440" s="3">
+      <c r="G440" s="6"/>
+      <c r="H440" s="8"/>
+      <c r="I440" s="6"/>
+      <c r="J440" s="8"/>
+      <c r="K440" s="6"/>
+      <c r="L440" s="8">
         <v>133</v>
       </c>
-      <c r="M440" s="1">
+      <c r="M440" s="9">
         <v>303000</v>
       </c>
-      <c r="T440" s="3" t="s">
+      <c r="N440" s="8"/>
+      <c r="O440" s="6"/>
+      <c r="P440" s="6"/>
+      <c r="Q440" s="8"/>
+      <c r="R440" s="8"/>
+      <c r="S440" s="8"/>
+      <c r="T440" s="8" t="s">
         <v>1205</v>
       </c>
       <c r="X440" t="s">
@@ -17408,20 +17735,31 @@
       <c r="C441" s="4">
         <v>15</v>
       </c>
-      <c r="D441" t="s">
+      <c r="D441" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E441" s="4" t="s">
+      <c r="E441" s="5" t="s">
         <v>835</v>
       </c>
-      <c r="F441" s="2" t="s">
+      <c r="F441" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L441" s="3">
+      <c r="G441" s="6"/>
+      <c r="H441" s="8"/>
+      <c r="I441" s="6"/>
+      <c r="J441" s="8"/>
+      <c r="K441" s="6"/>
+      <c r="L441" s="8">
         <v>211</v>
       </c>
-      <c r="M441" s="1"/>
-      <c r="T441" s="3" t="s">
+      <c r="M441" s="9"/>
+      <c r="N441" s="8"/>
+      <c r="O441" s="6"/>
+      <c r="P441" s="6"/>
+      <c r="Q441" s="8"/>
+      <c r="R441" s="8"/>
+      <c r="S441" s="8"/>
+      <c r="T441" s="8" t="s">
         <v>1206</v>
       </c>
       <c r="X441" t="s">
@@ -17432,20 +17770,31 @@
       <c r="C442" s="4">
         <v>16</v>
       </c>
-      <c r="D442" t="s">
+      <c r="D442" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E442" s="4" t="s">
+      <c r="E442" s="5" t="s">
         <v>836</v>
       </c>
-      <c r="F442" s="2" t="s">
+      <c r="F442" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L442" s="3">
+      <c r="G442" s="6"/>
+      <c r="H442" s="8"/>
+      <c r="I442" s="6"/>
+      <c r="J442" s="8"/>
+      <c r="K442" s="6"/>
+      <c r="L442" s="8">
         <v>115</v>
       </c>
-      <c r="M442" s="1"/>
-      <c r="T442" s="3" t="s">
+      <c r="M442" s="9"/>
+      <c r="N442" s="8"/>
+      <c r="O442" s="6"/>
+      <c r="P442" s="6"/>
+      <c r="Q442" s="8"/>
+      <c r="R442" s="8"/>
+      <c r="S442" s="8"/>
+      <c r="T442" s="8" t="s">
         <v>1207</v>
       </c>
       <c r="X442" t="s">
@@ -17456,20 +17805,31 @@
       <c r="C443" s="4">
         <v>17</v>
       </c>
-      <c r="D443" t="s">
+      <c r="D443" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E443" s="4" t="s">
+      <c r="E443" s="5" t="s">
         <v>837</v>
       </c>
-      <c r="F443" s="2" t="s">
+      <c r="F443" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L443" s="3">
+      <c r="G443" s="6"/>
+      <c r="H443" s="8"/>
+      <c r="I443" s="6"/>
+      <c r="J443" s="8"/>
+      <c r="K443" s="6"/>
+      <c r="L443" s="8">
         <v>170</v>
       </c>
-      <c r="M443" s="1"/>
-      <c r="T443" s="3" t="s">
+      <c r="M443" s="9"/>
+      <c r="N443" s="8"/>
+      <c r="O443" s="6"/>
+      <c r="P443" s="6"/>
+      <c r="Q443" s="8"/>
+      <c r="R443" s="8"/>
+      <c r="S443" s="8"/>
+      <c r="T443" s="8" t="s">
         <v>1208</v>
       </c>
       <c r="X443" t="s">
@@ -17480,20 +17840,31 @@
       <c r="C444" s="4">
         <v>18</v>
       </c>
-      <c r="D444" t="s">
+      <c r="D444" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E444" s="4" t="s">
+      <c r="E444" s="5" t="s">
         <v>839</v>
       </c>
-      <c r="F444" s="2" t="s">
+      <c r="F444" s="7" t="s">
         <v>838</v>
       </c>
-      <c r="L444" s="3">
+      <c r="G444" s="6"/>
+      <c r="H444" s="8"/>
+      <c r="I444" s="6"/>
+      <c r="J444" s="8"/>
+      <c r="K444" s="6"/>
+      <c r="L444" s="8">
         <v>253</v>
       </c>
-      <c r="M444" s="1"/>
-      <c r="T444" s="3" t="s">
+      <c r="M444" s="9"/>
+      <c r="N444" s="8"/>
+      <c r="O444" s="6"/>
+      <c r="P444" s="6"/>
+      <c r="Q444" s="8"/>
+      <c r="R444" s="8"/>
+      <c r="S444" s="8"/>
+      <c r="T444" s="8" t="s">
         <v>1209</v>
       </c>
       <c r="X444" t="s">
@@ -17504,22 +17875,33 @@
       <c r="C445" s="4">
         <v>19</v>
       </c>
-      <c r="D445" t="s">
+      <c r="D445" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E445" s="4" t="s">
+      <c r="E445" s="5" t="s">
         <v>840</v>
       </c>
-      <c r="F445" s="2" t="s">
+      <c r="F445" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="L445" s="3">
+      <c r="G445" s="6"/>
+      <c r="H445" s="8"/>
+      <c r="I445" s="6"/>
+      <c r="J445" s="8"/>
+      <c r="K445" s="6"/>
+      <c r="L445" s="8">
         <v>125</v>
       </c>
-      <c r="M445" s="1">
+      <c r="M445" s="9">
         <v>190000</v>
       </c>
-      <c r="T445" s="3" t="s">
+      <c r="N445" s="8"/>
+      <c r="O445" s="6"/>
+      <c r="P445" s="6"/>
+      <c r="Q445" s="8"/>
+      <c r="R445" s="8"/>
+      <c r="S445" s="8"/>
+      <c r="T445" s="8" t="s">
         <v>1210</v>
       </c>
       <c r="X445" t="s">

</xml_diff>

<commit_message>
added cars 12 - 14
</commit_message>
<xml_diff>
--- a/devData/H77Dyno.xlsx
+++ b/devData/H77Dyno.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\SQL\Halle77Dyno\devData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6537C363-ABE9-481D-8C36-2D2E16C0187E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F9DD3A-5731-4004-AA67-18A78615ACAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5168,13 +5168,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5367,19 +5367,19 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5738,8 +5738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="D396" sqref="D396:T396"/>
+    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="D339" sqref="D339:T339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5753,13 +5753,13 @@
     <col min="12" max="12" width="4.5703125" style="3" customWidth="1"/>
     <col min="14" max="14" width="8.7109375" style="3" customWidth="1"/>
     <col min="15" max="15" width="5.140625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="1.85546875" style="17" customWidth="1"/>
+    <col min="16" max="16" width="1.85546875" style="14" customWidth="1"/>
     <col min="17" max="17" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" style="11" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="1.7109375" style="18" customWidth="1"/>
+    <col min="19" max="19" width="1.7109375" style="15" customWidth="1"/>
     <col min="20" max="20" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="1.7109375" style="11" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="1.85546875" style="18" customWidth="1"/>
+    <col min="22" max="22" width="1.85546875" style="15" customWidth="1"/>
     <col min="23" max="23" width="2.140625" customWidth="1"/>
     <col min="24" max="24" width="4.7109375" customWidth="1"/>
     <col min="27" max="27" width="5.5703125" customWidth="1"/>
@@ -14574,16 +14574,29 @@
       <c r="C339" s="4">
         <v>1</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D339" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="E339" s="4" t="s">
+      <c r="E339" s="18" t="s">
         <v>951</v>
       </c>
-      <c r="L339" s="3">
+      <c r="F339" s="19"/>
+      <c r="G339" s="17"/>
+      <c r="H339" s="20"/>
+      <c r="I339" s="17"/>
+      <c r="J339" s="20"/>
+      <c r="K339" s="17"/>
+      <c r="L339" s="20">
         <v>192</v>
       </c>
-      <c r="T339" s="3" t="s">
+      <c r="M339" s="17"/>
+      <c r="N339" s="20"/>
+      <c r="O339" s="17"/>
+      <c r="P339" s="17"/>
+      <c r="Q339" s="20"/>
+      <c r="R339" s="20"/>
+      <c r="S339" s="20"/>
+      <c r="T339" s="20" t="s">
         <v>1299</v>
       </c>
       <c r="X339" t="s">
@@ -16149,33 +16162,33 @@
       <c r="C396" s="4">
         <v>1</v>
       </c>
-      <c r="D396" s="14" t="s">
+      <c r="D396" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E396" s="20">
+      <c r="E396" s="5">
         <v>944</v>
       </c>
-      <c r="F396" s="15" t="s">
+      <c r="F396" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="G396" s="14"/>
-      <c r="H396" s="16"/>
-      <c r="I396" s="14"/>
-      <c r="J396" s="16"/>
-      <c r="K396" s="14"/>
-      <c r="L396" s="16">
+      <c r="G396" s="6"/>
+      <c r="H396" s="8"/>
+      <c r="I396" s="6"/>
+      <c r="J396" s="8"/>
+      <c r="K396" s="6"/>
+      <c r="L396" s="8">
         <v>163</v>
       </c>
-      <c r="M396" s="14"/>
-      <c r="N396" s="16"/>
-      <c r="O396" s="14"/>
-      <c r="P396" s="14"/>
-      <c r="Q396" s="16" t="s">
+      <c r="M396" s="6"/>
+      <c r="N396" s="8"/>
+      <c r="O396" s="6"/>
+      <c r="P396" s="6"/>
+      <c r="Q396" s="8" t="s">
         <v>1232</v>
       </c>
-      <c r="R396" s="16"/>
-      <c r="S396" s="16"/>
-      <c r="T396" s="16"/>
+      <c r="R396" s="8"/>
+      <c r="S396" s="8"/>
+      <c r="T396" s="8"/>
       <c r="X396" t="s">
         <v>146</v>
       </c>
@@ -16184,22 +16197,33 @@
       <c r="C397" s="4">
         <v>2</v>
       </c>
-      <c r="D397" t="s">
+      <c r="D397" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E397" s="4" t="s">
+      <c r="E397" s="5" t="s">
         <v>865</v>
       </c>
-      <c r="F397" s="2" t="s">
+      <c r="F397" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="L397" s="3">
+      <c r="G397" s="6"/>
+      <c r="H397" s="8"/>
+      <c r="I397" s="6"/>
+      <c r="J397" s="8"/>
+      <c r="K397" s="6"/>
+      <c r="L397" s="8">
         <v>200</v>
       </c>
-      <c r="Q397" s="3" t="s">
+      <c r="M397" s="6"/>
+      <c r="N397" s="8"/>
+      <c r="O397" s="6"/>
+      <c r="P397" s="6"/>
+      <c r="Q397" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T397" s="3" t="s">
+      <c r="R397" s="8"/>
+      <c r="S397" s="8"/>
+      <c r="T397" s="8" t="s">
         <v>1236</v>
       </c>
       <c r="X397" t="s">
@@ -16219,25 +16243,35 @@
       <c r="C398" s="4">
         <v>3</v>
       </c>
-      <c r="D398" t="s">
+      <c r="D398" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E398" s="4" t="s">
+      <c r="E398" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="F398" s="2" t="s">
+      <c r="F398" s="7" t="s">
         <v>591</v>
       </c>
-      <c r="J398" s="3">
+      <c r="G398" s="6"/>
+      <c r="H398" s="8"/>
+      <c r="I398" s="6"/>
+      <c r="J398" s="8">
         <v>6</v>
       </c>
-      <c r="L398" s="3">
+      <c r="K398" s="6"/>
+      <c r="L398" s="8">
         <v>211</v>
       </c>
-      <c r="Q398" s="3" t="s">
+      <c r="M398" s="6"/>
+      <c r="N398" s="8"/>
+      <c r="O398" s="6"/>
+      <c r="P398" s="6"/>
+      <c r="Q398" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T398" s="3" t="s">
+      <c r="R398" s="8"/>
+      <c r="S398" s="8"/>
+      <c r="T398" s="8" t="s">
         <v>1237</v>
       </c>
       <c r="X398" t="s">
@@ -16257,25 +16291,35 @@
       <c r="C399" s="4">
         <v>4</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D399" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E399" s="4" t="s">
+      <c r="E399" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="F399" s="2" t="s">
+      <c r="F399" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L399" s="3">
+      <c r="G399" s="6"/>
+      <c r="H399" s="8"/>
+      <c r="I399" s="6"/>
+      <c r="J399" s="8"/>
+      <c r="K399" s="6"/>
+      <c r="L399" s="8">
         <v>180</v>
       </c>
-      <c r="M399" s="1">
+      <c r="M399" s="9">
         <v>300000</v>
       </c>
-      <c r="Q399" s="3" t="s">
+      <c r="N399" s="8"/>
+      <c r="O399" s="6"/>
+      <c r="P399" s="6"/>
+      <c r="Q399" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T399" s="3" t="s">
+      <c r="R399" s="8"/>
+      <c r="S399" s="8"/>
+      <c r="T399" s="8" t="s">
         <v>1238</v>
       </c>
       <c r="X399" t="s">
@@ -16286,22 +16330,33 @@
       <c r="C400" s="4">
         <v>5</v>
       </c>
-      <c r="D400" t="s">
+      <c r="D400" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E400" s="4" t="s">
+      <c r="E400" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="F400" s="2" t="s">
+      <c r="F400" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="L400" s="3">
+      <c r="G400" s="6"/>
+      <c r="H400" s="8"/>
+      <c r="I400" s="6"/>
+      <c r="J400" s="8"/>
+      <c r="K400" s="6"/>
+      <c r="L400" s="8">
         <v>204</v>
       </c>
-      <c r="Q400" s="3" t="s">
+      <c r="M400" s="6"/>
+      <c r="N400" s="8"/>
+      <c r="O400" s="6"/>
+      <c r="P400" s="6"/>
+      <c r="Q400" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T400" s="3" t="s">
+      <c r="R400" s="8"/>
+      <c r="S400" s="8"/>
+      <c r="T400" s="8" t="s">
         <v>1239</v>
       </c>
       <c r="X400" t="s">
@@ -16321,28 +16376,37 @@
       <c r="C401" s="4">
         <v>6</v>
       </c>
-      <c r="D401" t="s">
+      <c r="D401" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E401" s="4" t="s">
+      <c r="E401" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="F401" s="2" t="s">
+      <c r="F401" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G401" t="s">
+      <c r="G401" s="6" t="s">
         <v>873</v>
       </c>
-      <c r="J401" s="3">
+      <c r="H401" s="8"/>
+      <c r="I401" s="6"/>
+      <c r="J401" s="8">
         <v>6</v>
       </c>
-      <c r="L401" s="3">
+      <c r="K401" s="6"/>
+      <c r="L401" s="8">
         <v>150</v>
       </c>
-      <c r="Q401" s="3" t="s">
+      <c r="M401" s="6"/>
+      <c r="N401" s="8"/>
+      <c r="O401" s="6"/>
+      <c r="P401" s="6"/>
+      <c r="Q401" s="8" t="s">
         <v>1233</v>
       </c>
-      <c r="T401" s="3" t="s">
+      <c r="R401" s="8"/>
+      <c r="S401" s="8"/>
+      <c r="T401" s="8" t="s">
         <v>1240</v>
       </c>
       <c r="X401" t="s">
@@ -16353,22 +16417,33 @@
       <c r="C402" s="4">
         <v>7</v>
       </c>
-      <c r="D402" t="s">
+      <c r="D402" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E402" s="4" t="s">
+      <c r="E402" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F402" s="2" t="s">
+      <c r="F402" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="L402" s="3">
+      <c r="G402" s="6"/>
+      <c r="H402" s="8"/>
+      <c r="I402" s="6"/>
+      <c r="J402" s="8"/>
+      <c r="K402" s="6"/>
+      <c r="L402" s="8">
         <v>98</v>
       </c>
-      <c r="Q402" s="3" t="s">
+      <c r="M402" s="6"/>
+      <c r="N402" s="8"/>
+      <c r="O402" s="6"/>
+      <c r="P402" s="6"/>
+      <c r="Q402" s="8" t="s">
         <v>1234</v>
       </c>
-      <c r="T402" s="3" t="s">
+      <c r="R402" s="8"/>
+      <c r="S402" s="8"/>
+      <c r="T402" s="8" t="s">
         <v>1241</v>
       </c>
       <c r="X402" t="s">
@@ -16388,25 +16463,35 @@
       <c r="C403" s="4">
         <v>8</v>
       </c>
-      <c r="D403" t="s">
+      <c r="D403" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E403" s="4" t="s">
+      <c r="E403" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="F403" s="2" t="s">
+      <c r="F403" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G403" t="s">
+      <c r="G403" s="6" t="s">
         <v>565</v>
       </c>
-      <c r="L403" s="3">
+      <c r="H403" s="8"/>
+      <c r="I403" s="6"/>
+      <c r="J403" s="8"/>
+      <c r="K403" s="6"/>
+      <c r="L403" s="8">
         <v>290</v>
       </c>
-      <c r="Q403" s="3" t="s">
+      <c r="M403" s="6"/>
+      <c r="N403" s="8"/>
+      <c r="O403" s="6"/>
+      <c r="P403" s="6"/>
+      <c r="Q403" s="8" t="s">
         <v>1126</v>
       </c>
-      <c r="T403" s="3" t="s">
+      <c r="R403" s="8"/>
+      <c r="S403" s="8"/>
+      <c r="T403" s="8" t="s">
         <v>1242</v>
       </c>
       <c r="X403" t="s">
@@ -16426,25 +16511,35 @@
       <c r="C404" s="4">
         <v>9</v>
       </c>
-      <c r="D404" t="s">
+      <c r="D404" s="6" t="s">
         <v>878</v>
       </c>
-      <c r="E404" s="4" t="s">
+      <c r="E404" s="5" t="s">
         <v>879</v>
       </c>
-      <c r="F404" s="2" t="s">
+      <c r="F404" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H404" s="3" t="s">
+      <c r="G404" s="6"/>
+      <c r="H404" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L404" s="3">
+      <c r="I404" s="6"/>
+      <c r="J404" s="8"/>
+      <c r="K404" s="6"/>
+      <c r="L404" s="8">
         <v>140</v>
       </c>
-      <c r="Q404" s="3" t="s">
+      <c r="M404" s="6"/>
+      <c r="N404" s="8"/>
+      <c r="O404" s="6"/>
+      <c r="P404" s="6"/>
+      <c r="Q404" s="8" t="s">
         <v>1235</v>
       </c>
-      <c r="T404" s="3" t="s">
+      <c r="R404" s="8"/>
+      <c r="S404" s="8"/>
+      <c r="T404" s="8" t="s">
         <v>1243</v>
       </c>
       <c r="X404" t="s">
@@ -16455,22 +16550,33 @@
       <c r="C405" s="4">
         <v>10</v>
       </c>
-      <c r="D405" t="s">
+      <c r="D405" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E405" s="4" t="s">
+      <c r="E405" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="F405" s="2" t="s">
+      <c r="F405" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="L405" s="3">
+      <c r="G405" s="6"/>
+      <c r="H405" s="8"/>
+      <c r="I405" s="6"/>
+      <c r="J405" s="8"/>
+      <c r="K405" s="6"/>
+      <c r="L405" s="8">
         <v>136</v>
       </c>
-      <c r="N405" s="3">
+      <c r="M405" s="6"/>
+      <c r="N405" s="8">
         <v>1993</v>
       </c>
-      <c r="T405" s="3" t="s">
+      <c r="O405" s="6"/>
+      <c r="P405" s="6"/>
+      <c r="Q405" s="8"/>
+      <c r="R405" s="8"/>
+      <c r="S405" s="8"/>
+      <c r="T405" s="8" t="s">
         <v>1244</v>
       </c>
       <c r="X405" t="s">
@@ -16490,22 +16596,33 @@
       <c r="C406" s="4">
         <v>11</v>
       </c>
-      <c r="D406" t="s">
+      <c r="D406" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E406" s="4" t="s">
+      <c r="E406" s="5" t="s">
         <v>769</v>
       </c>
-      <c r="F406" s="2" t="s">
+      <c r="F406" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="H406" s="3" t="s">
+      <c r="G406" s="6"/>
+      <c r="H406" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="L406" s="3">
+      <c r="I406" s="6"/>
+      <c r="J406" s="8"/>
+      <c r="K406" s="6"/>
+      <c r="L406" s="8">
         <v>170</v>
       </c>
-      <c r="T406" s="3" t="s">
+      <c r="M406" s="6"/>
+      <c r="N406" s="8"/>
+      <c r="O406" s="6"/>
+      <c r="P406" s="6"/>
+      <c r="Q406" s="8"/>
+      <c r="R406" s="8"/>
+      <c r="S406" s="8"/>
+      <c r="T406" s="8" t="s">
         <v>1245</v>
       </c>
       <c r="X406" t="s">
@@ -16516,22 +16633,33 @@
       <c r="C407" s="4">
         <v>12</v>
       </c>
-      <c r="D407" t="s">
+      <c r="D407" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E407" s="4" t="s">
+      <c r="E407" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="F407" s="2" t="s">
+      <c r="F407" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="J407" s="3">
+      <c r="G407" s="6"/>
+      <c r="H407" s="8"/>
+      <c r="I407" s="6"/>
+      <c r="J407" s="8">
         <v>5</v>
       </c>
-      <c r="L407" s="3">
+      <c r="K407" s="6"/>
+      <c r="L407" s="8">
         <v>305</v>
       </c>
-      <c r="T407" s="3" t="s">
+      <c r="M407" s="6"/>
+      <c r="N407" s="8"/>
+      <c r="O407" s="6"/>
+      <c r="P407" s="6"/>
+      <c r="Q407" s="8"/>
+      <c r="R407" s="8"/>
+      <c r="S407" s="8"/>
+      <c r="T407" s="8" t="s">
         <v>1246</v>
       </c>
       <c r="X407" t="s">
@@ -16542,22 +16670,33 @@
       <c r="C408" s="4">
         <v>13</v>
       </c>
-      <c r="D408" t="s">
+      <c r="D408" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E408" s="4" t="s">
+      <c r="E408" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="F408" s="2" t="s">
+      <c r="F408" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="J408" s="3">
+      <c r="G408" s="6"/>
+      <c r="H408" s="8"/>
+      <c r="I408" s="6"/>
+      <c r="J408" s="8">
         <v>5</v>
       </c>
-      <c r="L408" s="3">
+      <c r="K408" s="6"/>
+      <c r="L408" s="8">
         <v>245</v>
       </c>
-      <c r="T408" s="3" t="s">
+      <c r="M408" s="6"/>
+      <c r="N408" s="8"/>
+      <c r="O408" s="6"/>
+      <c r="P408" s="6"/>
+      <c r="Q408" s="8"/>
+      <c r="R408" s="8"/>
+      <c r="S408" s="8"/>
+      <c r="T408" s="8" t="s">
         <v>1247</v>
       </c>
       <c r="X408" t="s">
@@ -18636,7 +18775,7 @@
       <c r="D465" s="6" t="s">
         <v>744</v>
       </c>
-      <c r="E465" s="19" t="s">
+      <c r="E465" s="16" t="s">
         <v>745</v>
       </c>
       <c r="F465" s="7" t="s">

</xml_diff>